<commit_message>
pridany template pro snimace
</commit_message>
<xml_diff>
--- a/instrumentace_template.xlsx
+++ b/instrumentace_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Skola - magistr\druhák\MPC-AUP\projekt\project_AUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0548158A-17F0-47CB-BE24-DD8DE7A0C991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18F7E86-9585-42FB-8063-17A3CC3E699E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5292" yWindow="0" windowWidth="17820" windowHeight="12360" xr2:uid="{3DF038C4-59DD-4D8C-89B0-4D36076B5952}"/>
+    <workbookView xWindow="7536" yWindow="0" windowWidth="18720" windowHeight="12360" xr2:uid="{3DF038C4-59DD-4D8C-89B0-4D36076B5952}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+  <si>
+    <t>Název</t>
+  </si>
+  <si>
+    <t>Snímače</t>
+  </si>
+  <si>
+    <t>Rozsah</t>
+  </si>
+  <si>
+    <t>Citlivost</t>
+  </si>
+  <si>
+    <t>Rozlišení</t>
+  </si>
+  <si>
+    <t>Provozní podmínky</t>
+  </si>
+  <si>
+    <t>Chyba měření</t>
+  </si>
+  <si>
+    <t>Mechanické vlastnosti</t>
+  </si>
+  <si>
+    <t>Rozhraní</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Odůvodnění</t>
+  </si>
+  <si>
+    <t>Porovnání parametrů</t>
+  </si>
+  <si>
+    <t>Provozní podminky</t>
+  </si>
+  <si>
+    <t>Porovnání</t>
+  </si>
+  <si>
+    <t>Označení</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -55,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -63,12 +113,234 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -383,14 +655,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D7AA1C-20CF-4490-A041-11CADF853C8E}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>2</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>3</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>4</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>5</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>6</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>